<commit_message>
Cambios V2V pedidos el 23-03-2023
</commit_message>
<xml_diff>
--- a/public/formatos/comercial/Ejemplo Base Comercial.xlsx
+++ b/public/formatos/comercial/Ejemplo Base Comercial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26322"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc6109987457ea29/Escritorio/CRM/Trafico comercial/Formatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_7B1621E403AB67B009FB721D2F85F5C55A3DFD15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89C8A394-FB21-4E13-B27D-2B5B966A133D}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="11_7B1621E403AB67B009FB721D2F85F5C55A3DFD15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{076CD7C9-4186-4FDA-BCB3-CAE105D9D4EA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Base" sheetId="1" r:id="rId1"/>
     <sheet name="Config" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,6 +25,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>FECHA</t>
   </si>
@@ -64,21 +66,60 @@
     <t>ESTADO</t>
   </si>
   <si>
+    <t>CUENTA</t>
+  </si>
+  <si>
     <t>F_INICIO</t>
   </si>
   <si>
     <t>DURA_MES</t>
   </si>
   <si>
+    <t>MASTERFOODS COLOMBIA LTDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VANS EXPERTO EN SONRISAS (SE DESCUENTA DEL SALDO DE MACA) </t>
+  </si>
+  <si>
+    <t>ALEJANDRO;50</t>
+  </si>
+  <si>
+    <t>LADY;50</t>
+  </si>
+  <si>
     <t>CERRADO</t>
   </si>
   <si>
+    <t>BULL MARKETING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEPSICO BEBIDAS </t>
+  </si>
+  <si>
+    <t>SEVEN ORIENTE (CRUCE CON SALDO ALEJANDRO LATIFF)</t>
+  </si>
+  <si>
+    <t>C3220204</t>
+  </si>
+  <si>
+    <t>LA ESQUINA DEL SABOR PEPSI (CRUCE CON SALDO ALEJANDRO LATIFF)</t>
+  </si>
+  <si>
+    <t>V2V</t>
+  </si>
+  <si>
+    <t>KELLOGS DE COLOMBIA</t>
+  </si>
+  <si>
+    <t>TARJETAS BANCOLOMBIA 2FASE  (SE FACTURO POR ADELANTADO)</t>
+  </si>
+  <si>
+    <t>COTIZACION</t>
+  </si>
+  <si>
     <t>EJECUCIONXFACTURAR</t>
   </si>
   <si>
-    <t>COTIZACION</t>
-  </si>
-  <si>
     <t>PERDIDO</t>
   </si>
   <si>
@@ -89,36 +130,6 @@
   </si>
   <si>
     <t>VENTAEJECUCION</t>
-  </si>
-  <si>
-    <t>MASTERFOODS COLOMBIA LTDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VANS EXPERTO EN SONRISAS (SE DESCUENTA DEL SALDO DE MACA) </t>
-  </si>
-  <si>
-    <t>ALEJANDRO;50</t>
-  </si>
-  <si>
-    <t>LADY;50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEPSICO BEBIDAS </t>
-  </si>
-  <si>
-    <t>SEVEN ORIENTE (CRUCE CON SALDO ALEJANDRO LATIFF)</t>
-  </si>
-  <si>
-    <t>C3220204</t>
-  </si>
-  <si>
-    <t>LA ESQUINA DEL SABOR PEPSI (CRUCE CON SALDO ALEJANDRO LATIFF)</t>
-  </si>
-  <si>
-    <t>KELLOGS DE COLOMBIA</t>
-  </si>
-  <si>
-    <t>TARJETAS BANCOLOMBIA 2FASE  (SE FACTURO POR ADELANTADO)</t>
   </si>
 </sst>
 </file>
@@ -135,7 +146,7 @@
     <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="171" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -170,13 +181,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -262,11 +266,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -355,64 +359,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person10.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person11.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person12.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person6.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person7.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person8.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person9.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -700,7 +648,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -708,25 +656,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="19.109375" customWidth="1"/>
-    <col min="19" max="19" width="20.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="20" max="20" width="20.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="9" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -754,110 +701,122 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="10"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
+      <c r="L1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="10"/>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="11">
         <v>44982</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="12">
+        <v>128658571</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="11">
+        <v>44986</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="13">
-        <v>128658571</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E3" s="12">
+        <v>209530413</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="11">
+        <v>44988</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
-        <v>44986</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E4" s="12">
+        <v>28982980</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="11">
+        <v>44994</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="13">
-        <v>209530413</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
-        <v>44988</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="13">
-        <v>28982980</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
-        <v>44994</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
       </c>
       <c r="D5">
         <v>69220301</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>62507774</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -866,12 +825,18 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD110AE5-3B52-4AF9-A1E8-8A351CD66A4F}">
           <x14:formula1>
             <xm:f>Config!$A$1:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0CFB424E-4C9A-43B0-9080-470027556559}">
+          <x14:formula1>
+            <xm:f>Config!$C$1:$C$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -881,47 +846,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8996F2E4-A3C4-4E12-A452-C076478F35E9}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="C1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>